<commit_message>
merged readme documents to readme.md and replaced one file with anonymised version
</commit_message>
<xml_diff>
--- a/Valuation Template_DRC.xlsx
+++ b/Valuation Template_DRC.xlsx
@@ -320,7 +320,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+If construction period is 12 months, enter 6 in this cell</t>
         </r>
       </text>
     </comment>
@@ -699,27 +699,6 @@
     <t>Leasehold</t>
   </si>
   <si>
-    <t>Jo Carter MRICS</t>
-  </si>
-  <si>
-    <t>Louise Attwood MRICS</t>
-  </si>
-  <si>
-    <t>Nick Keyse</t>
-  </si>
-  <si>
-    <t>Scott Ramsay MRICS</t>
-  </si>
-  <si>
-    <t>Rhys Griffiths MRICS</t>
-  </si>
-  <si>
-    <t>Gareth King</t>
-  </si>
-  <si>
-    <t>Steve Williams MRICS</t>
-  </si>
-  <si>
     <t>psf (NIA)</t>
   </si>
   <si>
@@ -816,9 +795,6 @@
     <t>Notes as to how obsolescence was considered must be included here.  Need to  consider Physical / Functional / Economic and External obsolescence.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ben Winstanley </t>
-  </si>
-  <si>
     <t>Total Gross cost including finance</t>
   </si>
   <si>
@@ -838,6 +814,30 @@
   </si>
   <si>
     <t>NB: For assets of more than £Xm only where a single component exceeds Y% of the value of the asset</t>
+  </si>
+  <si>
+    <t>NAME1</t>
+  </si>
+  <si>
+    <t>NAME2</t>
+  </si>
+  <si>
+    <t>NAME3</t>
+  </si>
+  <si>
+    <t>NAME4</t>
+  </si>
+  <si>
+    <t>NAME5</t>
+  </si>
+  <si>
+    <t>NAME6</t>
+  </si>
+  <si>
+    <t>NAME7</t>
+  </si>
+  <si>
+    <t>NAME8</t>
   </si>
 </sst>
 </file>
@@ -1633,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1650,7 +1650,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="77" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="19"/>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -1846,19 +1846,19 @@
     </row>
     <row r="19" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="23"/>
       <c r="D19" s="98" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E19" s="98"/>
       <c r="F19" s="99"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="23"/>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="1"/>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="1"/>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="80" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D24" s="81"/>
       <c r="E24" s="81"/>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="32" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="97" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B32" s="97"/>
       <c r="C32" s="97"/>
@@ -1986,25 +1986,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="56" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D35" s="61"/>
       <c r="E35" s="56" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D36" s="27"/>
       <c r="E36" s="56" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="39" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C37" s="51"/>
       <c r="D37" t="s">
@@ -2025,7 +2025,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="52" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="40" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="F45" s="95"/>
       <c r="G45" s="57" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H45" s="58"/>
     </row>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="56" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D48">
         <f>D36</f>
@@ -2154,14 +2154,14 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E54" s="59"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="68"/>
       <c r="B55" s="56" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F55" s="60">
         <f>(((1+E54)^(A55/12))*F53)-F53</f>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="69" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F56" s="60">
         <f>F53+F55</f>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="56" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D64" s="29"/>
     </row>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="69" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="74" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B69" s="75"/>
       <c r="C69" s="75"/>
@@ -2274,17 +2274,17 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="56" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="56" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2385,7 +2385,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2460,74 +2460,74 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="39" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="39" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="39" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2536,7 +2536,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="39" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B32" s="39" t="s">
         <v>12</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="39" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B33" s="39" t="s">
         <v>13</v>
@@ -2552,17 +2552,17 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="39" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="39" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added "checked by" field
</commit_message>
<xml_diff>
--- a/Valuation Template_DRC.xlsx
+++ b/Valuation Template_DRC.xlsx
@@ -21,7 +21,7 @@
     <author>Carter, Jo</author>
   </authors>
   <commentList>
-    <comment ref="C10" authorId="0">
+    <comment ref="C11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,19 +43,6 @@
           <t xml:space="preserve">
 If not inspected state that it was a desktop valuation
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Must match summary spreadsheet</t>
         </r>
       </text>
     </comment>
@@ -68,12 +55,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Must match summary spreadsheet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="14"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>In case of PPE only 
 Must match summary spreadsheet</t>
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0">
+    <comment ref="C20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="0">
+    <comment ref="D37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C37" authorId="0">
+    <comment ref="C38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A40" authorId="0">
+    <comment ref="A41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D45" authorId="0">
+    <comment ref="D46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0">
+    <comment ref="F46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -276,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="0">
+    <comment ref="C47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A55" authorId="0">
+    <comment ref="A56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C58" authorId="0">
+    <comment ref="C59" authorId="0">
       <text>
         <r>
           <rPr>
@@ -471,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F60" authorId="0">
+    <comment ref="F61" authorId="0">
       <text>
         <r>
           <rPr>
@@ -499,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D64" authorId="0">
+    <comment ref="D65" authorId="0">
       <text>
         <r>
           <rPr>
@@ -529,7 +529,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
   <si>
     <t>UPRN:</t>
   </si>
@@ -838,6 +838,9 @@
   </si>
   <si>
     <t>NAME8</t>
+  </si>
+  <si>
+    <t>Checked by:</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1142,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1320,6 +1323,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1631,10 +1635,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1706,7 +1710,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
@@ -1718,57 +1722,57 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="26" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="4"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1776,147 +1780,151 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="C14" s="7"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="73"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="18"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="73"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="22">
+      <c r="B18" s="8"/>
+      <c r="C18" s="22">
+        <f>F68</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="46">
         <f>F67</f>
         <v>0</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="46">
-        <f>F66</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="100" t="s">
+      <c r="D19" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="100"/>
-      <c r="F18" s="101"/>
-    </row>
-    <row r="19" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="E19" s="100"/>
+      <c r="F19" s="101"/>
+    </row>
+    <row r="20" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="98" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="98"/>
-      <c r="F19" s="99"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="99"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="10"/>
+        <v>67</v>
+      </c>
+      <c r="B22" s="8"/>
       <c r="C22" s="1"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="89" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="91"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="91"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="80" t="s">
+      <c r="B25" s="10"/>
+      <c r="C25" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="82"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="85"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="82"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
@@ -1959,95 +1967,95 @@
       <c r="F30" s="85"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="88"/>
-    </row>
-    <row r="32" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="97" t="s">
+      <c r="A31" s="3"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="85"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="88"/>
+    </row>
+    <row r="33" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="97" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="40" t="s">
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
-    </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="40"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="27"/>
+      <c r="D36" s="61"/>
       <c r="E36" s="56" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="51"/>
-      <c r="D37" t="s">
+      <c r="C38" s="51"/>
+      <c r="D38" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="28">
-        <f>C37*2.47</f>
+      <c r="E38" s="28">
+        <f>C38*2.47</f>
         <v>0</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="39"/>
-      <c r="C38" s="31"/>
-      <c r="E38" s="28"/>
-    </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="39"/>
+      <c r="C39" s="31"/>
+      <c r="E39" s="28"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="55"/>
-    </row>
-    <row r="40" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="92"/>
-      <c r="B40" s="93"/>
-      <c r="C40" s="93"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="94"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="49"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="55"/>
+    </row>
+    <row r="41" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="92"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="94"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="49"/>
@@ -2058,251 +2066,259 @@
       <c r="F42" s="49"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="49"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="32"/>
-      <c r="E45" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" s="95"/>
-      <c r="G45" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="H45" s="58"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="32"/>
+      <c r="E46" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="95"/>
+      <c r="G46" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" s="58"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="63">
-        <f>D45*C46</f>
+      <c r="C47" s="51"/>
+      <c r="D47" s="63">
+        <f>D46*C47</f>
         <v>0</v>
       </c>
-      <c r="E46" s="43" t="s">
+      <c r="E47" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="96"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F47" s="39"/>
+      <c r="F47" s="96"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="56" t="s">
+      <c r="F48" s="39"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="D48">
-        <f>D36</f>
+      <c r="D49">
+        <f>D37</f>
         <v>0</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="63">
-        <f>D46*D48</f>
+      <c r="D50" s="63">
+        <f>D47*D49</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="39" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="66"/>
-      <c r="D50" s="65">
-        <f>D49*C50</f>
+      <c r="C51" s="66"/>
+      <c r="D51" s="65">
+        <f>D50*C51</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F51" s="63">
-        <f>D49+D50</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="67"/>
-      <c r="D52" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F52" s="64">
-        <f>F51*C52</f>
+      <c r="F52" s="63">
+        <f>D50+D51</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="67"/>
+      <c r="D53" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="64">
+        <f>F52*C53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="63">
-        <f>F51+F52</f>
+      <c r="F54" s="63">
+        <f>F52+F53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>76</v>
       </c>
-      <c r="E54" s="59"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="68"/>
-      <c r="B55" s="56" t="s">
+      <c r="E55" s="59"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="68"/>
+      <c r="B56" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="F55" s="60">
-        <f>(((1+E54)^(A55/12))*F53)-F53</f>
+      <c r="F56" s="60">
+        <f>(((1+E55)^(A56/12))*F54)-F54</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="69" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="F56" s="60">
-        <f>F53+F55</f>
+      <c r="F57" s="60">
+        <f>F54+F56</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="39"/>
-      <c r="F57" s="33"/>
-    </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="39"/>
+      <c r="F58" s="33"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="34"/>
-      <c r="D58" s="35"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C59" s="34"/>
       <c r="D59" s="35"/>
-      <c r="E59" s="36" t="s">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D60" s="35"/>
+      <c r="E60" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="F59" s="70">
-        <f>ROUND((F56-(F56*C58)),-3)</f>
+      <c r="F60" s="70">
+        <f>ROUND((F57-(F57*C59)),-3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E60" s="36" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E61" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F60" s="44"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="40" t="s">
+      <c r="F61" s="44"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="39" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D63" s="71"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="56" t="s">
+      <c r="D64" s="71"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="D64" s="29"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D65" s="37"/>
-    </row>
-    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D66" s="30"/>
-      <c r="E66" s="41" t="s">
+      <c r="D65" s="29"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D66" s="37"/>
+    </row>
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D67" s="30"/>
+      <c r="E67" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="F66" s="62">
-        <f>ROUND((D63*D64),-3)</f>
+      <c r="F67" s="62">
+        <f>ROUND((D64*D65),-3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="E67" s="41" t="s">
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="E68" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F67" s="45">
-        <f>F59+F66</f>
+      <c r="F68" s="45">
+        <f>F60+F67</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E68" s="17"/>
-      <c r="F68" s="38"/>
-    </row>
-    <row r="69" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="74" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E69" s="17"/>
+      <c r="F69" s="38"/>
+    </row>
+    <row r="70" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="B69" s="75"/>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="76"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
+      <c r="B70" s="75"/>
+      <c r="C70" s="75"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="75"/>
+      <c r="F70" s="76"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="56" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="56" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A70:F70"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C24:F31"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="C25:F32"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E46" display="http://service.bcis.co.uk"/>
+    <hyperlink ref="E47" display="http://service.bcis.co.uk"/>
   </hyperlinks>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -2318,49 +2334,49 @@
           <x14:formula1>
             <xm:f>'Dropdown lists'!$A$5:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C11</xm:sqref>
+          <xm:sqref>C12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dropdown lists'!$A$9:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C12</xm:sqref>
+          <xm:sqref>C13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dropdown lists'!$A$39:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>C22 C20</xm:sqref>
+          <xm:sqref>C23 C21</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dropdown lists'!$A$35:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>C21</xm:sqref>
+          <xm:sqref>C22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dropdown lists'!$A$18:$A$25</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>C7:C8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dropdown lists'!$A$14:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>C13</xm:sqref>
+          <xm:sqref>C14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dropdown lists'!$B$32:$B$33</xm:f>
           </x14:formula1>
-          <xm:sqref>E63</xm:sqref>
+          <xm:sqref>E64</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dropdown lists'!$A$32:$A$33</xm:f>
           </x14:formula1>
-          <xm:sqref>B64</xm:sqref>
+          <xm:sqref>B65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Reverting document to original
Corrected Test Changes incorporated on website by mistake
</commit_message>
<xml_diff>
--- a/Valuation Template_DRC.xlsx
+++ b/Valuation Template_DRC.xlsx
@@ -529,7 +529,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
   <si>
     <t>UPRN:</t>
   </si>
@@ -840,10 +840,7 @@
     <t>Checked by:</t>
   </si>
   <si>
-    <t>?????????????</t>
-  </si>
-  <si>
-    <t>Test 2</t>
+    <t>Insert property name</t>
   </si>
 </sst>
 </file>
@@ -1640,8 +1637,8 @@
   </sheetPr>
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1657,7 +1654,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -1684,9 +1681,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="20"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
-        <v>103</v>
-      </c>
+      <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>

</xml_diff>

<commit_message>
Removal of question marks that were used as a test
I removed question marks in cell E5 (or near to it) that were used
previously to test the github process.
</commit_message>
<xml_diff>
--- a/Valuation Template_DRC.xlsx
+++ b/Valuation Template_DRC.xlsx
@@ -529,7 +529,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
   <si>
     <t>UPRN:</t>
   </si>
@@ -841,9 +841,6 @@
   </si>
   <si>
     <t>&lt;Insert property name&gt;</t>
-  </si>
-  <si>
-    <t>????????</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1638,7 @@
   <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1696,9 +1693,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="19"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>

</xml_diff>